<commit_message>
gnerdmaster - cambios varios (underline strikethrough)
</commit_message>
<xml_diff>
--- a/Exports/test01.xlsx
+++ b/Exports/test01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gofelixc\source\repos\InteropExcel\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A9F7FF-A9DB-430D-9AD4-04A955C750FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2685C2-FDC1-4C38-824E-3F66652F15E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C8DB73DC-C0FF-4ECA-B124-CAC5C056723F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{550859BB-2993-43DF-8755-A923E96CAA33}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Sin formato</t>
   </si>
@@ -165,6 +165,39 @@
   </si>
   <si>
     <t>font-style: underline-double bold italic</t>
+  </si>
+  <si>
+    <t>font-style: strikethrough</t>
+  </si>
+  <si>
+    <t>font-style: line-through</t>
+  </si>
+  <si>
+    <t>font-style: strikethrough italic</t>
+  </si>
+  <si>
+    <t>font-style: line-through bold</t>
+  </si>
+  <si>
+    <t>strikethrough: True</t>
+  </si>
+  <si>
+    <t>text-decoration-line: strikethrough</t>
+  </si>
+  <si>
+    <t>text-decoration-line: line-through</t>
+  </si>
+  <si>
+    <t>text-decoration-line: strikethrough underline</t>
+  </si>
+  <si>
+    <t>text-decoration-line: line-through underline</t>
+  </si>
+  <si>
+    <t>text-decoration-line: line-through underline-double</t>
+  </si>
+  <si>
+    <t>text-decoration-style: solid</t>
   </si>
   <si>
     <t>color: red</t>
@@ -184,7 +217,7 @@
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="165" formatCode="??\=??"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +269,50 @@
     <font>
       <b/>
       <i/>
+      <u val="double"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <u val="double"/>
       <sz val="12"/>
       <color theme="1"/>
@@ -774,7 +851,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -920,23 +997,38 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1252,19 +1344,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B22181-6A09-4894-AA93-C3EBF19DE806}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542C6021-4D54-4A7C-985D-4A3065400B35}">
   <dimension ref="B1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="2"/>
-    <col min="7" max="7" width="121.28515625" customWidth="1"/>
-    <col min="9" max="9" width="41.7109375" customWidth="1"/>
+    <col min="7" max="7" width="116" customWidth="1"/>
+    <col min="9" max="9" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1274,7 +1366,7 @@
       <c r="I1" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="51"/>
+      <c r="J1" s="56"/>
     </row>
     <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -1288,8 +1380,8 @@
         <v>34</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="M2" s="55" t="s">
-        <v>43</v>
+      <c r="M2" s="60" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1301,8 +1393,8 @@
         <v>35</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="M3" s="56" t="s">
-        <v>44</v>
+      <c r="M3" s="61" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1316,8 +1408,8 @@
         <v>36</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="M4" s="57" t="s">
-        <v>45</v>
+      <c r="M4" s="62" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1338,8 +1430,8 @@
       <c r="I6" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
     </row>
     <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
@@ -1350,8 +1442,8 @@
       <c r="I7" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
     </row>
     <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G8" s="18" t="s">
@@ -1360,8 +1452,8 @@
       <c r="I8" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -1373,8 +1465,8 @@
       <c r="I9" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
     </row>
     <row r="10" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G10" s="19" t="s">
@@ -1383,8 +1475,8 @@
       <c r="I10" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
     </row>
     <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="str">
@@ -1394,8 +1486,8 @@
       <c r="I11" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
     </row>
     <row r="12" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="str">
@@ -1407,15 +1499,18 @@
       <c r="G12" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-    </row>
-    <row r="13" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+    </row>
+    <row r="13" spans="2:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
+      <c r="I13" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
     </row>
     <row r="14" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
@@ -1424,12 +1519,18 @@
       <c r="G14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-    </row>
-    <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
+      <c r="I14" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+    </row>
+    <row r="15" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
     </row>
     <row r="16" spans="2:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
@@ -1440,15 +1541,21 @@
       <c r="G16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
+      <c r="I16" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="58"/>
+      <c r="K16" s="58"/>
     </row>
     <row r="17" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
+      <c r="I17" s="51" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="58"/>
+      <c r="K17" s="58"/>
     </row>
     <row r="18" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="12"/>
@@ -1457,12 +1564,18 @@
       <c r="G18" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
+      <c r="I18" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="58"/>
+      <c r="K18" s="58"/>
     </row>
     <row r="19" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
+      <c r="I19" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="58"/>
+      <c r="K19" s="58"/>
     </row>
     <row r="20" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
@@ -1473,13 +1586,19 @@
       <c r="G20" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="53"/>
-      <c r="K20" s="53"/>
-    </row>
-    <row r="21" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="58"/>
+      <c r="K20" s="58"/>
+    </row>
+    <row r="21" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
+      <c r="I21" s="54" t="s">
+        <v>51</v>
+      </c>
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
       <c r="L21" s="32"/>
@@ -1491,11 +1610,17 @@
       <c r="G22" s="25" t="s">
         <v>18</v>
       </c>
+      <c r="I22" s="55" t="s">
+        <v>52</v>
+      </c>
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
       <c r="L22" s="32"/>
     </row>
-    <row r="23" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23" s="47" t="s">
+        <v>53</v>
+      </c>
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>

</xml_diff>

<commit_message>
gnerdmaster - added option shrink-to-fit (reducir para ajustar texto
</commit_message>
<xml_diff>
--- a/Exports/test01.xlsx
+++ b/Exports/test01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gofelixc\source\repos\InteropExcel\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2685C2-FDC1-4C38-824E-3F66652F15E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7756F4-D795-46D9-8F9B-882B70148759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{550859BB-2993-43DF-8755-A923E96CAA33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F299BBA-ED69-49BD-B1F9-0334C9AC2EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Sin formato</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>TEST ALIGNMENT</t>
+  </si>
+  <si>
+    <t>shrink-to-fit:true(encoge contenido)</t>
+  </si>
+  <si>
+    <t>shrink:true(encoge contenido)</t>
+  </si>
+  <si>
+    <t>shrinktofit:true</t>
   </si>
   <si>
     <t>WrapText - Este es un test de un texto demasiado largo, y tiene que pasar la prueba de Wrap text = Ajustar texto</t>
@@ -217,7 +226,7 @@
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="165" formatCode="??\=??"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,14 +245,6 @@
       <b/>
       <i/>
       <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u val="doubleAccounting"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -851,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -880,8 +881,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -988,12 +993,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1009,26 +1014,23 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1344,44 +1346,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542C6021-4D54-4A7C-985D-4A3065400B35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E795889F-D9B2-4723-A8FA-205B7E00CB3F}">
   <dimension ref="B1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="2"/>
-    <col min="7" max="7" width="116" customWidth="1"/>
-    <col min="9" max="9" width="54.140625" customWidth="1"/>
+    <col min="7" max="7" width="118.85546875" customWidth="1"/>
+    <col min="9" max="9" width="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="56"/>
+        <v>10</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="57"/>
     </row>
     <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="G2" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>34</v>
+      <c r="G2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="45" t="s">
+        <v>37</v>
       </c>
       <c r="J2" s="2"/>
-      <c r="M2" s="60" t="s">
-        <v>54</v>
+      <c r="M2" s="61" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1389,27 +1389,27 @@
         <v>1</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="I3" s="44" t="s">
-        <v>35</v>
+      <c r="I3" s="46" t="s">
+        <v>38</v>
       </c>
       <c r="J3" s="2"/>
-      <c r="M3" s="61" t="s">
-        <v>55</v>
+      <c r="M3" s="62" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>43831</v>
       </c>
-      <c r="G4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="45" t="s">
-        <v>36</v>
+      <c r="G4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="47" t="s">
+        <v>39</v>
       </c>
       <c r="J4" s="2"/>
-      <c r="M4" s="62" t="s">
-        <v>56</v>
+      <c r="M4" s="63" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -1419,19 +1419,19 @@
       <c r="C5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="2:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="G6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
+      <c r="G6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
     </row>
     <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
@@ -1439,21 +1439,21 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="I7" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
+      <c r="I7" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
     </row>
     <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
+      <c r="G8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
     </row>
     <row r="9" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -1462,267 +1462,273 @@
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="I9" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
+      <c r="I9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
     </row>
     <row r="10" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G10" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
+      <c r="B10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
     </row>
     <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="str">
+      <c r="B11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="58"/>
+      <c r="K11" s="58"/>
+    </row>
+    <row r="12" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+    </row>
+    <row r="13" spans="2:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="str">
         <f>_xlfn.CONCAT("TEST", " PARA UNA FUNCIÓN")</f>
         <v>TEST PARA UNA FUNCIÓN</v>
       </c>
-      <c r="I11" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-    </row>
-    <row r="12" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="str">
+      <c r="I13" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+    </row>
+    <row r="14" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="str">
         <f>_xlfn.CONCAT("TEST", " PARA UNA FUNCIÓN EN CELDA CONVINADA")</f>
         <v>TEST PARA UNA FUNCIÓN EN CELDA CONVINADA</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="G12" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-    </row>
-    <row r="13" spans="2:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="I13" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-    </row>
-    <row r="14" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="G14" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
+      <c r="G14" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
     </row>
     <row r="15" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I15" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
+      <c r="B15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="I15" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
     </row>
     <row r="16" spans="2:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="G16" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="53" t="s">
-        <v>46</v>
-      </c>
-      <c r="J16" s="58"/>
-      <c r="K16" s="58"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="G16" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
     </row>
     <row r="17" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="I17" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17" s="58"/>
-      <c r="K17" s="58"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="I17" s="52" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
     </row>
     <row r="18" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="G18" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="J18" s="58"/>
-      <c r="K18" s="58"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="G18" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
     </row>
     <row r="19" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I19" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="J19" s="58"/>
-      <c r="K19" s="58"/>
+      <c r="I19" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
     </row>
     <row r="20" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="G20" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="J20" s="58"/>
-      <c r="K20" s="58"/>
+      <c r="B20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="G20" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
     </row>
     <row r="21" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="I21" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="I21" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
     </row>
     <row r="22" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="G22" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="G22" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="56" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
     </row>
     <row r="23" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I23" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
+      <c r="I23" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
     </row>
     <row r="24" spans="2:12" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G24" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
+      <c r="G24" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
     </row>
     <row r="25" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G26" s="27" t="s">
-        <v>20</v>
+      <c r="G26" s="29" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G28" s="28" t="s">
-        <v>21</v>
+      <c r="G28" s="30" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="29" t="s">
-        <v>22</v>
+      <c r="G30" s="31" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="2:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G32" s="30" t="s">
-        <v>23</v>
+      <c r="G32" s="32" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="7:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G34" s="31" t="s">
-        <v>24</v>
+      <c r="G34" s="33" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="7:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G36" s="33" t="s">
-        <v>25</v>
+      <c r="G36" s="35" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="7:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G38" s="34" t="s">
-        <v>26</v>
+      <c r="G38" s="36" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G40" s="35" t="s">
-        <v>27</v>
+      <c r="G40" s="37" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G42" s="36" t="s">
-        <v>28</v>
+      <c r="G42" s="38" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G44" s="37" t="s">
-        <v>29</v>
+      <c r="G44" s="39" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="7:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G46" s="38" t="s">
-        <v>30</v>
+      <c r="G46" s="40" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="7:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="7:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G48" s="39" t="s">
-        <v>31</v>
+      <c r="G48" s="41" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="7:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="50" spans="7:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G50" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H50" s="40"/>
+      <c r="G50" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="H50" s="42"/>
     </row>
     <row r="51" spans="7:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G51" s="40"/>
-      <c r="H51" s="40"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="42"/>
     </row>
     <row r="52" spans="7:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G52" s="40"/>
-      <c r="H52" s="40"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="42"/>
     </row>
     <row r="53" spans="7:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="43"/>
     </row>
     <row r="54" spans="7:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B12:D14"/>
-    <mergeCell ref="B16:D18"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D18"/>
     <mergeCell ref="B20:D22"/>
     <mergeCell ref="F1:F1048576"/>
     <mergeCell ref="J1:J5"/>

</xml_diff>

<commit_message>
gnerdmaster - added text-transform: lowercase | uppercase | capitalize | none
</commit_message>
<xml_diff>
--- a/Exports/test01.xlsx
+++ b/Exports/test01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gofelixc\source\repos\InteropExcel\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7756F4-D795-46D9-8F9B-882B70148759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA515CFE-A961-4106-8D47-C020CAD77D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F299BBA-ED69-49BD-B1F9-0334C9AC2EBB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B9641174-89A3-4FF3-8F06-1D565242BA8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Sin formato</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>color: rgb(174, 241, 71)</t>
+  </si>
+  <si>
+    <t>tExT-tRaNsFoRm: none</t>
+  </si>
+  <si>
+    <t>TEXT-TRANSFORM: UPPERCASE</t>
+  </si>
+  <si>
+    <t>text-transform: lowercase</t>
+  </si>
+  <si>
+    <t>Text-Transform: Capitalize</t>
   </si>
 </sst>
 </file>
@@ -1346,20 +1358,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E795889F-D9B2-4723-A8FA-205B7E00CB3F}">
-  <dimension ref="B1:M54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379C6055-EC34-4F2F-AE31-51C2E9E3225B}">
+  <dimension ref="B1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="2"/>
-    <col min="7" max="7" width="118.85546875" customWidth="1"/>
-    <col min="9" max="9" width="51" customWidth="1"/>
+    <col min="7" max="7" width="132.42578125" customWidth="1"/>
+    <col min="9" max="9" width="54.42578125" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
+    <col min="14" max="14" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1367,8 +1383,11 @@
         <v>36</v>
       </c>
       <c r="J1" s="57"/>
-    </row>
-    <row r="2" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N1" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1383,8 +1402,11 @@
       <c r="M2" s="61" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N2" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1396,8 +1418,11 @@
       <c r="M3" s="62" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N3" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="4">
         <v>43831</v>
       </c>
@@ -1411,15 +1436,18 @@
       <c r="M4" s="63" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N4" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>5123</v>
       </c>
       <c r="C5" s="2"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1433,7 +1461,7 @@
       <c r="J6" s="58"/>
       <c r="K6" s="58"/>
     </row>
-    <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1445,7 +1473,7 @@
       <c r="J7" s="58"/>
       <c r="K7" s="58"/>
     </row>
-    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G8" s="20" t="s">
         <v>14</v>
       </c>
@@ -1455,7 +1483,7 @@
       <c r="J8" s="58"/>
       <c r="K8" s="58"/>
     </row>
-    <row r="9" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
@@ -1468,7 +1496,7 @@
       <c r="J9" s="58"/>
       <c r="K9" s="58"/>
     </row>
-    <row r="10" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>5</v>
       </c>
@@ -1481,7 +1509,7 @@
       <c r="J10" s="58"/>
       <c r="K10" s="58"/>
     </row>
-    <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
         <v>6</v>
       </c>
@@ -1491,7 +1519,7 @@
       <c r="J11" s="58"/>
       <c r="K11" s="58"/>
     </row>
-    <row r="12" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="12" t="s">
         <v>7</v>
       </c>
@@ -1501,7 +1529,7 @@
       <c r="J12" s="60"/>
       <c r="K12" s="60"/>
     </row>
-    <row r="13" spans="2:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="str">
         <f>_xlfn.CONCAT("TEST", " PARA UNA FUNCIÓN")</f>
         <v>TEST PARA UNA FUNCIÓN</v>
@@ -1512,7 +1540,7 @@
       <c r="J13" s="60"/>
       <c r="K13" s="60"/>
     </row>
-    <row r="14" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="str">
         <f>_xlfn.CONCAT("TEST", " PARA UNA FUNCIÓN EN CELDA CONVINADA")</f>
         <v>TEST PARA UNA FUNCIÓN EN CELDA CONVINADA</v>
@@ -1528,7 +1556,7 @@
       <c r="J14" s="60"/>
       <c r="K14" s="60"/>
     </row>
-    <row r="15" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="13" t="s">
         <v>8</v>
       </c>
@@ -1540,7 +1568,7 @@
       <c r="J15" s="60"/>
       <c r="K15" s="60"/>
     </row>
-    <row r="16" spans="2:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>

</xml_diff>